<commit_message>
update collocations and essays
</commit_message>
<xml_diff>
--- a/Mispronounced words.xlsx
+++ b/Mispronounced words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer\个人资料\English\English Note\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CD2BB8-67A2-4492-919D-0083834A002E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DDCA69-8CA6-41BB-92F0-A9D6225AFAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +103,24 @@
   </si>
   <si>
     <t>/ˈkraɪ.sɪs/</t>
+  </si>
+  <si>
+    <t>theoretical</t>
+  </si>
+  <si>
+    <t>/θɪəˈret.ɪ.kəl/</t>
+  </si>
+  <si>
+    <t>理论上的</t>
+  </si>
+  <si>
+    <t>part of speech</t>
+  </si>
+  <si>
+    <t>meaning</t>
+  </si>
+  <si>
+    <t>[n.] [v.]</t>
   </si>
 </sst>
 </file>
@@ -155,10 +173,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="hair">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -167,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -175,10 +199,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -459,122 +484,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A12" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" ht="16.5" customHeight="1">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" ht="16.5" customHeight="1">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" ht="16.5" customHeight="1">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" ht="16.5" customHeight="1">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" ht="16.5" customHeight="1">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" ht="16.5" customHeight="1">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" ht="16.5" customHeight="1">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" ht="16.5" customHeight="1">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" ht="16.5" customHeight="1">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" ht="16.5" customHeight="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>